<commit_message>
get PSAF into rq134 table
</commit_message>
<xml_diff>
--- a/dashboard-ui/src/components/Research/variables/Variable Definitions RQ134_PH2.xlsx
+++ b/dashboard-ui/src/components/Research/variables/Variable Definitions RQ134_PH2.xlsx
@@ -190,7 +190,7 @@
     <t>Levels</t>
   </si>
   <si>
-    <t>Phase 2 - P2E_June_2025</t>
+    <t>P2E_June_2025, P2E_July_2025, P2E_Sept_2025</t>
   </si>
   <si>
     <t>Military, Civilian, emailParticipant, Online</t>
@@ -205,7 +205,7 @@
     <t>1-21</t>
   </si>
   <si>
-    <t>Affiliation Focus (AF), Merit Focus (MF), Personal Safety (PS), Search vs. Stay (SS), and Affiliation Focus / Merit Focus (AF-MF)</t>
+    <t>Affiliation Focus (AF), Merit Focus (MF), Personal Safety (PS), Search vs. Stay (SS), Affiliation Focus / Merit Focus (AF-MF), Personal Safety / Affiliation Focus (PS-AF)</t>
   </si>
   <si>
     <t>1-3</t>
@@ -643,7 +643,7 @@
     <col min="28" max="28" style="3" width="19.290714285714284" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="33" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="31.5" customFormat="1" s="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -729,7 +729,7 @@
         <v>27</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="46.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="44.25" customFormat="1" s="1">
       <c r="A2" s="2" t="s">
         <v>28</v>
       </c>
@@ -815,7 +815,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="181.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="171.75" customFormat="1" s="1">
       <c r="A3" s="2" t="s">
         <v>34</v>
       </c>
@@ -897,7 +897,7 @@
         <v>50</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="154.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="146.25" customFormat="1" s="1">
       <c r="A4" s="2" t="s">
         <v>57</v>
       </c>

</xml_diff>

<commit_message>
updated variable definitions for september rq134
</commit_message>
<xml_diff>
--- a/dashboard-ui/src/components/Research/variables/Variable Definitions RQ134_PH2.xlsx
+++ b/dashboard-ui/src/components/Research/variables/Variable Definitions RQ134_PH2.xlsx
@@ -190,7 +190,7 @@
     <t>Levels</t>
   </si>
   <si>
-    <t>P2E_June_2025, P2E_July_2025, P2E_Sept_2025</t>
+    <t>P2E_June_2025, P2E_July_2025</t>
   </si>
   <si>
     <t>Military, Civilian, emailParticipant, Online</t>
@@ -205,7 +205,7 @@
     <t>1-21</t>
   </si>
   <si>
-    <t>Affiliation Focus (AF), Merit Focus (MF), Personal Safety (PS), Search vs. Stay (SS), Affiliation Focus / Merit Focus (AF-MF), Personal Safety / Affiliation Focus (PS-AF)</t>
+    <t>Affiliation Focus (AF), Merit Focus (MF), Personal Safety (PS), Search vs. Stay (SS), Affiliation Focus / Merit Focus (AF-MF)</t>
   </si>
   <si>
     <t>1-3</t>
@@ -897,7 +897,7 @@
         <v>50</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="146.25" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="159" customFormat="1" s="1">
       <c r="A4" s="2" t="s">
         <v>57</v>
       </c>

</xml_diff>

<commit_message>
Update RQ134 for september eval (#357)
* started updating rq134 table for september eval ph2

* get PSAF into rq134 table

* more rq134 september progress

* got all rows to show up for every participant

* sort targets properly

* added alignment comparison to rq134 for september eval

* updated variable definitions for september rq134

* display both comparison scores

* update 'delegation' to 'delegation preference'

---------

Co-authored-by: dereknop <dereknop@gmail.com>
</commit_message>
<xml_diff>
--- a/dashboard-ui/src/components/Research/variables/Variable Definitions RQ134_PH2.xlsx
+++ b/dashboard-ui/src/components/Research/variables/Variable Definitions RQ134_PH2.xlsx
@@ -190,7 +190,7 @@
     <t>Levels</t>
   </si>
   <si>
-    <t>Phase 2 - P2E_June_2025</t>
+    <t>P2E_June_2025, P2E_July_2025</t>
   </si>
   <si>
     <t>Military, Civilian, emailParticipant, Online</t>
@@ -205,7 +205,7 @@
     <t>1-21</t>
   </si>
   <si>
-    <t>Affiliation Focus (AF), Merit Focus (MF), Personal Safety (PS), Search vs. Stay (SS), and Affiliation Focus / Merit Focus (AF-MF)</t>
+    <t>Affiliation Focus (AF), Merit Focus (MF), Personal Safety (PS), Search vs. Stay (SS), Affiliation Focus / Merit Focus (AF-MF)</t>
   </si>
   <si>
     <t>1-3</t>
@@ -643,7 +643,7 @@
     <col min="28" max="28" style="3" width="19.290714285714284" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="33" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="31.5" customFormat="1" s="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -729,7 +729,7 @@
         <v>27</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="46.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="44.25" customFormat="1" s="1">
       <c r="A2" s="2" t="s">
         <v>28</v>
       </c>
@@ -815,7 +815,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="181.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="171.75" customFormat="1" s="1">
       <c r="A3" s="2" t="s">
         <v>34</v>
       </c>
@@ -897,7 +897,7 @@
         <v>50</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="154.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="159" customFormat="1" s="1">
       <c r="A4" s="2" t="s">
         <v>57</v>
       </c>

</xml_diff>